<commit_message>
Actualización de datos de de Bug report
</commit_message>
<xml_diff>
--- a/Diseño y ejecución/BugReport_WilliamCabrera.xlsx
+++ b/Diseño y ejecución/BugReport_WilliamCabrera.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WILLIAM\Documents\WILLIAM\QA_AUTOMATION\AUTOMATIZACIÓN\PROYECTO DE AUTOMATIZACIÓN\PLAN DE PRUEBAS Y CASO DE PRUEBAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WILLIAM\Documents\workspace\proyec_petStore\Diseño y ejecución\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6562777C-8519-4AE3-8AE2-8CB3C39E2D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EDA1B7-6312-4264-A275-C6767729D86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Identificador</t>
   </si>
@@ -145,28 +145,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Al poner un valor no valido en la categiria </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t>neme</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Poppins"/>
-      </rPr>
-      <t xml:space="preserve"> me da un Status code 200 Ok</t>
-    </r>
-  </si>
-  <si>
     <t>Se debe mostrar un Status code 405 invalid input como respuesta de que el valor ingresado no es correcto</t>
   </si>
   <si>
@@ -183,6 +161,389 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1EJKB8Oq37nQ2vyqja7KPhxbr01HPMBm6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>PS_BG002</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> de la mascota admite tipo entero cuando solo debe de admitir tipo string</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al poner un valor no valido en la categiria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> da un Status code 200 Ok</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al poner un valor no valido en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">  de la mascota da un Status code 200 Ok</t>
+    </r>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14KjYz0dh9OiwXQ1n2YqDsSd58iZ1tXgt/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>PS_BG003</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> de la mascota admite tipo entero cuando solo debe de admitir tipo string</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Hecer clic en request  POST Add a new pet to the store
+2. Ir a la opción Body
+3. Cabiar el campus obligatoria de nombre de la mascota por núemeros enteros (234)
+4. Click en el botón </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">send </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>para correr el codigo JSON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Hecer clic en request  POST Add a new pet to the store
+2. Ir a la opción Body
+3. Cabiar el campus obligatoria de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> de la mascota por núemeros enteros (234)
+4. Click en el botón </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">send </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>para correr el codigo JSON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al poner un valor no valido en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">  de la mascota da un Status code 200 Ok</t>
+    </r>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1b8Q6fiLc73g30Jhmc2sny2F46VRZQuNh/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>PS_BG004</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al dejar el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> de la categoria, el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> de la mascota o el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> vacio no beria ejcutarse el codigo hasta que tenga datos validos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Hecer clic en request  POST Add a new pet to the store
+2. Ir a la opción Body
+3. Dejar vacio el campus obligatoria de la categoria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve"> el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">de la mascota o el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>status.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">
+4. Click en el botón send para correr el codigo JSON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al dejar cualquier campus vacio como la categiria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">de la mascota o es </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t xml:space="preserve">status </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Poppins"/>
+      </rPr>
+      <t>de la macota da un Status code 200 Ok</t>
+    </r>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1HE71bz0GILc1LCj-57CkuCdErIW8hvA7?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -248,7 +609,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -266,19 +627,6 @@
       <top style="dotted">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="dotted">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="dotted">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
@@ -304,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -328,13 +676,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -558,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -573,6 +918,7 @@
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -620,41 +966,41 @@
     </row>
     <row r="3" spans="1:28" ht="156" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -672,20 +1018,44 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="156" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="B4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
@@ -702,20 +1072,44 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="156" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
@@ -732,20 +1126,44 @@
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
     </row>
-    <row r="6" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="156" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="B6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -762,7 +1180,7 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
@@ -792,7 +1210,7 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -5922,9 +6340,12 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" xr:uid="{C24035A5-C5C0-4E26-A9CD-8FDCFF79593C}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{5015E05C-5C3A-4F31-A977-89CDE38DFE59}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{8F8C2FCF-0D58-4A68-AD13-1B7B15688392}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{1D66B677-A2CF-4928-B3EA-7FC407B174C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>